<commit_message>
changes from shreyas 1
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumPractice\HelixKTLO\HelixV2E\src\test\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13580" windowHeight="1780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10730" windowHeight="3580"/>
   </bookViews>
   <sheets>
     <sheet name="sanityTest" sheetId="2" r:id="rId1"/>
@@ -24,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">prodSanityTest!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1136" uniqueCount="303">
   <si>
     <t>applicationname</t>
   </si>
@@ -936,6 +932,12 @@
   </si>
   <si>
     <t>diptifff@gmail.com</t>
+  </si>
+  <si>
+    <t>https://ltes-hx.ie1.qa2b.affiniongroup.com/?source=SPAIHOMEPG0002</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> jonsyx@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1258,15 +1260,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1278,6 +1271,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1594,10 +1605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1811,7 +1822,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="39" t="s">
+      <c r="A11" s="36" t="s">
         <v>298</v>
       </c>
       <c r="B11" s="33" t="s">
@@ -1820,13 +1831,33 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="40" t="s">
+      <c r="D11" s="37" t="s">
         <v>300</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="42" t="s">
+      <c r="F11" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="43" t="s">
+        <v>302</v>
+      </c>
+      <c r="E12" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="39" t="s">
         <v>289</v>
       </c>
     </row>
@@ -1850,9 +1881,10 @@
     <hyperlink ref="B10" r:id="rId16"/>
     <hyperlink ref="B11" r:id="rId17"/>
     <hyperlink ref="D11" r:id="rId18" display="mailto:diptifff@gmail.com"/>
+    <hyperlink ref="B12" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -3868,10 +3900,10 @@
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -3882,7 +3914,7 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="40" t="s">
         <v>87</v>
       </c>
       <c r="H28" s="21" t="s">
@@ -3891,8 +3923,8 @@
       <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="38"/>
-      <c r="B29" s="38"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="10" t="s">
         <v>40</v>
       </c>
@@ -3901,17 +3933,17 @@
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="36"/>
+      <c r="G29" s="40"/>
       <c r="H29" s="21" t="s">
         <v>41</v>
       </c>
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="41" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -3922,7 +3954,7 @@
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="36" t="s">
+      <c r="G30" s="40" t="s">
         <v>88</v>
       </c>
       <c r="H30" s="21" t="s">
@@ -3931,8 +3963,8 @@
       <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="38"/>
-      <c r="B31" s="38"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="10" t="s">
         <v>40</v>
       </c>
@@ -3941,7 +3973,7 @@
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="36"/>
+      <c r="G31" s="40"/>
       <c r="H31" s="21" t="s">
         <v>41</v>
       </c>
@@ -4575,10 +4607,10 @@
       <c r="I58" s="21"/>
     </row>
     <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="37" t="s">
+      <c r="B59" s="41" t="s">
         <v>145</v>
       </c>
       <c r="C59" s="10" t="s">
@@ -4589,7 +4621,7 @@
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="36" t="s">
+      <c r="G59" s="40" t="s">
         <v>145</v>
       </c>
       <c r="H59" s="21" t="s">
@@ -4598,8 +4630,8 @@
       <c r="I59" s="21"/>
     </row>
     <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="38"/>
-      <c r="B60" s="38"/>
+      <c r="A60" s="42"/>
+      <c r="B60" s="42"/>
       <c r="C60" s="10" t="s">
         <v>40</v>
       </c>
@@ -4608,7 +4640,7 @@
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="36"/>
+      <c r="G60" s="40"/>
       <c r="H60" s="21" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
one more client and code change
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumPractice\HelixKTLO\HelixV2E\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10730" windowHeight="3580"/>
   </bookViews>
@@ -19,7 +24,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">prodSanityTest!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1057,7 +1061,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1142,17 +1146,6 @@
       <top style="medium">
         <color rgb="FFC1C7D0"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1269,8 +1262,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1281,14 +1280,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1608,7 +1601,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1837,12 +1830,12 @@
       <c r="E11" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="45" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="41" t="s">
         <v>112</v>
       </c>
       <c r="B12" s="33" t="s">
@@ -1851,13 +1844,13 @@
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="39" t="s">
         <v>302</v>
       </c>
-      <c r="E12" s="44" t="s">
+      <c r="E12" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="45" t="s">
         <v>289</v>
       </c>
     </row>
@@ -3900,10 +3893,10 @@
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="43" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -3914,7 +3907,7 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="40" t="s">
+      <c r="G28" s="42" t="s">
         <v>87</v>
       </c>
       <c r="H28" s="21" t="s">
@@ -3923,8 +3916,8 @@
       <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="42"/>
-      <c r="B29" s="42"/>
+      <c r="A29" s="44"/>
+      <c r="B29" s="44"/>
       <c r="C29" s="10" t="s">
         <v>40</v>
       </c>
@@ -3933,17 +3926,17 @@
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="40"/>
+      <c r="G29" s="42"/>
       <c r="H29" s="21" t="s">
         <v>41</v>
       </c>
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="43" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -3954,7 +3947,7 @@
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="42" t="s">
         <v>88</v>
       </c>
       <c r="H30" s="21" t="s">
@@ -3963,8 +3956,8 @@
       <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="44"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="10" t="s">
         <v>40</v>
       </c>
@@ -3973,7 +3966,7 @@
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="40"/>
+      <c r="G31" s="42"/>
       <c r="H31" s="21" t="s">
         <v>41</v>
       </c>
@@ -4607,10 +4600,10 @@
       <c r="I58" s="21"/>
     </row>
     <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="41" t="s">
+      <c r="A59" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="43" t="s">
         <v>145</v>
       </c>
       <c r="C59" s="10" t="s">
@@ -4621,7 +4614,7 @@
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="40" t="s">
+      <c r="G59" s="42" t="s">
         <v>145</v>
       </c>
       <c r="H59" s="21" t="s">
@@ -4630,8 +4623,8 @@
       <c r="I59" s="21"/>
     </row>
     <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="42"/>
-      <c r="B60" s="42"/>
+      <c r="A60" s="44"/>
+      <c r="B60" s="44"/>
       <c r="C60" s="10" t="s">
         <v>40</v>
       </c>
@@ -4640,7 +4633,7 @@
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="40"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="21" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
comment by change in one file
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeleniumPractice\HelixKTLO\HelixV2E\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10730" windowHeight="3580"/>
   </bookViews>
@@ -19,7 +24,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">prodSanityTest!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1088,7 +1092,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1176,23 +1180,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1307,9 +1300,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1655,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1664,7 +1654,7 @@
     <col min="1" max="1" width="30.36328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="74.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" style="48" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" style="47" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1759,7 +1749,7 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="43" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -1779,7 +1769,7 @@
       <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -1799,7 +1789,7 @@
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="44" t="s">
+      <c r="D7" s="43" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -1819,7 +1809,7 @@
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="44" t="s">
+      <c r="D8" s="43" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -1859,7 +1849,7 @@
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="44" t="s">
         <v>297</v>
       </c>
       <c r="E10" s="35" t="s">
@@ -1879,7 +1869,7 @@
       <c r="C11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="45" t="s">
         <v>300</v>
       </c>
       <c r="E11" s="37" t="s">
@@ -1899,7 +1889,7 @@
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="46" t="s">
         <v>302</v>
       </c>
       <c r="E12" s="39" t="s">
@@ -1910,7 +1900,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="56" x14ac:dyDescent="0.35">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="42" t="s">
         <v>303</v>
       </c>
       <c r="B13" s="33" t="s">
@@ -1925,8 +1915,8 @@
       <c r="E13" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="42" t="s">
-        <v>14</v>
+      <c r="F13" s="41" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1939,14 +1929,14 @@
       <c r="C14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="48" t="s">
         <v>307</v>
       </c>
       <c r="E14" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="42" t="s">
-        <v>14</v>
+      <c r="F14" s="41" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -1959,13 +1949,13 @@
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="48" t="s">
         <v>310</v>
       </c>
       <c r="E15" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="41" t="s">
         <v>289</v>
       </c>
     </row>
@@ -1979,14 +1969,14 @@
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="48" t="s">
         <v>312</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="42" t="s">
-        <v>14</v>
+      <c r="F16" s="41" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>
@@ -4036,10 +4026,10 @@
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B28" s="51" t="s">
+      <c r="B28" s="50" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="10" t="s">
@@ -4050,7 +4040,7 @@
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="50" t="s">
+      <c r="G28" s="49" t="s">
         <v>87</v>
       </c>
       <c r="H28" s="21" t="s">
@@ -4059,8 +4049,8 @@
       <c r="I28" s="21"/>
     </row>
     <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="52"/>
-      <c r="B29" s="52"/>
+      <c r="A29" s="51"/>
+      <c r="B29" s="51"/>
       <c r="C29" s="10" t="s">
         <v>40</v>
       </c>
@@ -4069,17 +4059,17 @@
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="50"/>
+      <c r="G29" s="49"/>
       <c r="H29" s="21" t="s">
         <v>41</v>
       </c>
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B30" s="51" t="s">
+      <c r="B30" s="50" t="s">
         <v>88</v>
       </c>
       <c r="C30" s="10" t="s">
@@ -4090,7 +4080,7 @@
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="50" t="s">
+      <c r="G30" s="49" t="s">
         <v>88</v>
       </c>
       <c r="H30" s="21" t="s">
@@ -4099,8 +4089,8 @@
       <c r="I30" s="21"/>
     </row>
     <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="52"/>
-      <c r="B31" s="52"/>
+      <c r="A31" s="51"/>
+      <c r="B31" s="51"/>
       <c r="C31" s="10" t="s">
         <v>40</v>
       </c>
@@ -4109,7 +4099,7 @@
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="50"/>
+      <c r="G31" s="49"/>
       <c r="H31" s="21" t="s">
         <v>41</v>
       </c>
@@ -4743,10 +4733,10 @@
       <c r="I58" s="21"/>
     </row>
     <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="51" t="s">
+      <c r="A59" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="51" t="s">
+      <c r="B59" s="50" t="s">
         <v>145</v>
       </c>
       <c r="C59" s="10" t="s">
@@ -4757,7 +4747,7 @@
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="20"/>
-      <c r="G59" s="50" t="s">
+      <c r="G59" s="49" t="s">
         <v>145</v>
       </c>
       <c r="H59" s="21" t="s">
@@ -4766,8 +4756,8 @@
       <c r="I59" s="21"/>
     </row>
     <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="52"/>
-      <c r="B60" s="52"/>
+      <c r="A60" s="51"/>
+      <c r="B60" s="51"/>
       <c r="C60" s="10" t="s">
         <v>40</v>
       </c>
@@ -4776,7 +4766,7 @@
       </c>
       <c r="E60" s="8"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="50"/>
+      <c r="G60" s="49"/>
       <c r="H60" s="21" t="s">
         <v>41</v>
       </c>

</xml_diff>